<commit_message>
goals are always plotted above shots
</commit_message>
<xml_diff>
--- a/Table predictions/E0/2017-08-28 - End of GW3/2017-08-28.xlsx
+++ b/Table predictions/E0/2017-08-28 - End of GW3/2017-08-28.xlsx
@@ -86,10 +86,10 @@
     <t>West Ham</t>
   </si>
   <si>
+    <t>Watford</t>
+  </si>
+  <si>
     <t>Crystal Palace</t>
-  </si>
-  <si>
-    <t>Watford</t>
   </si>
   <si>
     <t>Swansea</t>
@@ -509,7 +509,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,25 +549,25 @@
         <v>8</v>
       </c>
       <c r="B2" s="4">
-        <v>23.84</v>
+        <v>23.85</v>
       </c>
       <c r="C2" s="4">
-        <v>7.46</v>
+        <v>7.43</v>
       </c>
       <c r="D2" s="4">
-        <v>6.7</v>
+        <v>6.72</v>
       </c>
       <c r="E2" s="4">
-        <v>78.97</v>
+        <v>78.98</v>
       </c>
       <c r="F2" s="4">
-        <v>38.54</v>
+        <v>38.49</v>
       </c>
       <c r="G2" s="4">
-        <v>40.380000000000003</v>
+        <v>40.020000000000003</v>
       </c>
       <c r="H2" s="4">
-        <v>89.89</v>
+        <v>90.32</v>
       </c>
       <c r="I2" s="4">
         <v>0</v>
@@ -578,25 +578,25 @@
         <v>9</v>
       </c>
       <c r="B3" s="6">
-        <v>22.63</v>
+        <v>22.6</v>
       </c>
       <c r="C3" s="6">
-        <v>7.28</v>
+        <v>7.25</v>
       </c>
       <c r="D3" s="6">
-        <v>8.09</v>
+        <v>8.15</v>
       </c>
       <c r="E3" s="6">
-        <v>75.17</v>
+        <v>75.040000000000006</v>
       </c>
       <c r="F3" s="6">
-        <v>35.700000000000003</v>
+        <v>35.46</v>
       </c>
       <c r="G3" s="6">
-        <v>19.39</v>
+        <v>19.03</v>
       </c>
       <c r="H3" s="6">
-        <v>77.42</v>
+        <v>76.959999999999994</v>
       </c>
       <c r="I3" s="6">
         <v>0</v>
@@ -607,25 +607,25 @@
         <v>10</v>
       </c>
       <c r="B4" s="6">
-        <v>22.11</v>
+        <v>22.07</v>
       </c>
       <c r="C4" s="6">
-        <v>7.57</v>
+        <v>7.61</v>
       </c>
       <c r="D4" s="6">
         <v>8.32</v>
       </c>
       <c r="E4" s="6">
-        <v>73.89</v>
+        <v>73.83</v>
       </c>
       <c r="F4" s="6">
-        <v>32.85</v>
+        <v>32.82</v>
       </c>
       <c r="G4" s="6">
-        <v>16.36</v>
+        <v>15.81</v>
       </c>
       <c r="H4" s="6">
-        <v>73.319999999999993</v>
+        <v>72.53</v>
       </c>
       <c r="I4" s="6">
         <v>0</v>
@@ -636,25 +636,25 @@
         <v>11</v>
       </c>
       <c r="B5" s="6">
-        <v>21.61</v>
+        <v>21.68</v>
       </c>
       <c r="C5" s="6">
-        <v>7.7</v>
+        <v>7.64</v>
       </c>
       <c r="D5" s="6">
-        <v>8.69</v>
+        <v>8.68</v>
       </c>
       <c r="E5" s="6">
-        <v>72.540000000000006</v>
+        <v>72.69</v>
       </c>
       <c r="F5" s="6">
         <v>31.1</v>
       </c>
       <c r="G5" s="6">
-        <v>10.5</v>
+        <v>11.23</v>
       </c>
       <c r="H5" s="6">
-        <v>64.42</v>
+        <v>65.02</v>
       </c>
       <c r="I5" s="6">
         <v>0</v>
@@ -665,25 +665,25 @@
         <v>12</v>
       </c>
       <c r="B6" s="8">
-        <v>21.64</v>
+        <v>21.63</v>
       </c>
       <c r="C6" s="8">
-        <v>7.33</v>
+        <v>7.35</v>
       </c>
       <c r="D6" s="8">
         <v>9.02</v>
       </c>
       <c r="E6" s="8">
-        <v>72.260000000000005</v>
+        <v>72.239999999999995</v>
       </c>
       <c r="F6" s="8">
-        <v>28.09</v>
+        <v>28.01</v>
       </c>
       <c r="G6" s="8">
-        <v>12.18</v>
+        <v>12.58</v>
       </c>
       <c r="H6" s="8">
-        <v>66.69</v>
+        <v>65.94</v>
       </c>
       <c r="I6" s="8">
         <v>0</v>
@@ -694,28 +694,28 @@
         <v>13</v>
       </c>
       <c r="B7" s="8">
-        <v>18.350000000000001</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="C7" s="8">
-        <v>6.56</v>
+        <v>6.59</v>
       </c>
       <c r="D7" s="8">
-        <v>13.09</v>
+        <v>12.99</v>
       </c>
       <c r="E7" s="8">
-        <v>61.6</v>
+        <v>61.86</v>
       </c>
       <c r="F7" s="8">
-        <v>11.55</v>
+        <v>11.87</v>
       </c>
       <c r="G7" s="8">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="H7" s="8">
-        <v>14.89</v>
+        <v>15.23</v>
       </c>
       <c r="I7" s="8">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -726,22 +726,22 @@
         <v>16.13</v>
       </c>
       <c r="C8" s="8">
-        <v>9.24</v>
+        <v>9.23</v>
       </c>
       <c r="D8" s="8">
-        <v>12.63</v>
+        <v>12.64</v>
       </c>
       <c r="E8" s="8">
-        <v>57.64</v>
+        <v>57.62</v>
       </c>
       <c r="F8" s="8">
-        <v>6.96</v>
+        <v>6.89</v>
       </c>
       <c r="G8" s="8">
         <v>0.22</v>
       </c>
       <c r="H8" s="8">
-        <v>5.32</v>
+        <v>5.54</v>
       </c>
       <c r="I8" s="8">
         <v>0.17</v>
@@ -752,28 +752,28 @@
         <v>15</v>
       </c>
       <c r="B9" s="8">
-        <v>16.3</v>
+        <v>16.38</v>
       </c>
       <c r="C9" s="8">
-        <v>8.4</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="D9" s="8">
-        <v>13.3</v>
+        <v>13.32</v>
       </c>
       <c r="E9" s="8">
-        <v>57.29</v>
+        <v>57.44</v>
       </c>
       <c r="F9" s="8">
-        <v>5.75</v>
+        <v>5.9</v>
       </c>
       <c r="G9" s="8">
-        <v>0.21</v>
+        <v>0.16</v>
       </c>
       <c r="H9" s="8">
-        <v>5.05</v>
+        <v>5.53</v>
       </c>
       <c r="I9" s="8">
-        <v>0.28999999999999998</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -781,28 +781,28 @@
         <v>16</v>
       </c>
       <c r="B10" s="8">
-        <v>14.81</v>
+        <v>14.79</v>
       </c>
       <c r="C10" s="8">
         <v>8.56</v>
       </c>
       <c r="D10" s="8">
-        <v>14.63</v>
+        <v>14.65</v>
       </c>
       <c r="E10" s="8">
-        <v>53</v>
+        <v>52.93</v>
       </c>
       <c r="F10" s="8">
-        <v>-2.11</v>
+        <v>-2.12</v>
       </c>
       <c r="G10" s="8">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H10" s="8">
-        <v>1.39</v>
+        <v>1.44</v>
       </c>
       <c r="I10" s="8">
-        <v>1.1399999999999999</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -810,28 +810,28 @@
         <v>17</v>
       </c>
       <c r="B11" s="8">
-        <v>14.47</v>
+        <v>14.41</v>
       </c>
       <c r="C11" s="8">
-        <v>8.26</v>
+        <v>8.25</v>
       </c>
       <c r="D11" s="8">
-        <v>15.27</v>
+        <v>15.34</v>
       </c>
       <c r="E11" s="8">
-        <v>51.66</v>
+        <v>51.47</v>
       </c>
       <c r="F11" s="8">
-        <v>-2.04</v>
+        <v>-2.36</v>
       </c>
       <c r="G11" s="8">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="H11" s="8">
-        <v>1.04</v>
+        <v>0.85</v>
       </c>
       <c r="I11" s="8">
-        <v>1.67</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -839,28 +839,28 @@
         <v>18</v>
       </c>
       <c r="B12" s="8">
-        <v>13.75</v>
+        <v>13.72</v>
       </c>
       <c r="C12" s="8">
-        <v>6.91</v>
+        <v>6.97</v>
       </c>
       <c r="D12" s="8">
-        <v>17.34</v>
+        <v>17.309999999999999</v>
       </c>
       <c r="E12" s="8">
-        <v>48.16</v>
+        <v>48.14</v>
       </c>
       <c r="F12" s="8">
-        <v>-7.47</v>
+        <v>-7.37</v>
       </c>
       <c r="G12" s="8">
         <v>0</v>
       </c>
       <c r="H12" s="8">
-        <v>0.38</v>
+        <v>0.35</v>
       </c>
       <c r="I12" s="8">
-        <v>4.99</v>
+        <v>5.72</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -868,28 +868,28 @@
         <v>19</v>
       </c>
       <c r="B13" s="8">
-        <v>12.6</v>
+        <v>12.64</v>
       </c>
       <c r="C13" s="8">
-        <v>7.07</v>
+        <v>7.04</v>
       </c>
       <c r="D13" s="8">
-        <v>18.329999999999998</v>
+        <v>18.309999999999999</v>
       </c>
       <c r="E13" s="8">
-        <v>44.88</v>
+        <v>44.97</v>
       </c>
       <c r="F13" s="8">
-        <v>-14.82</v>
+        <v>-14.66</v>
       </c>
       <c r="G13" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H13" s="8">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="I13" s="8">
-        <v>10.28</v>
+        <v>11.34</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -897,19 +897,19 @@
         <v>20</v>
       </c>
       <c r="B14" s="8">
-        <v>12.09</v>
+        <v>11.76</v>
       </c>
       <c r="C14" s="8">
-        <v>7.22</v>
+        <v>9.32</v>
       </c>
       <c r="D14" s="8">
-        <v>18.690000000000001</v>
+        <v>16.920000000000002</v>
       </c>
       <c r="E14" s="8">
-        <v>43.49</v>
+        <v>44.61</v>
       </c>
       <c r="F14" s="8">
-        <v>-14.56</v>
+        <v>-12.04</v>
       </c>
       <c r="G14" s="8">
         <v>0</v>
@@ -918,7 +918,7 @@
         <v>0.03</v>
       </c>
       <c r="I14" s="8">
-        <v>15.92</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -926,28 +926,28 @@
         <v>21</v>
       </c>
       <c r="B15" s="8">
-        <v>11.28</v>
+        <v>12.09</v>
       </c>
       <c r="C15" s="8">
-        <v>9.09</v>
+        <v>7.24</v>
       </c>
       <c r="D15" s="8">
-        <v>16.63</v>
+        <v>18.670000000000002</v>
       </c>
       <c r="E15" s="8">
-        <v>42.93</v>
+        <v>43.51</v>
       </c>
       <c r="F15" s="8">
-        <v>-12.54</v>
+        <v>-14.49</v>
       </c>
       <c r="G15" s="8">
         <v>0</v>
       </c>
       <c r="H15" s="8">
-        <v>0.02</v>
+        <v>0.12</v>
       </c>
       <c r="I15" s="8">
-        <v>15.47</v>
+        <v>16.32</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -955,28 +955,28 @@
         <v>22</v>
       </c>
       <c r="B16" s="8">
-        <v>11.19</v>
+        <v>11.24</v>
       </c>
       <c r="C16" s="8">
-        <v>8.01</v>
+        <v>8</v>
       </c>
       <c r="D16" s="8">
-        <v>18.8</v>
+        <v>18.760000000000002</v>
       </c>
       <c r="E16" s="8">
-        <v>41.57</v>
+        <v>41.72</v>
       </c>
       <c r="F16" s="8">
-        <v>-19.8</v>
+        <v>-19.53</v>
       </c>
       <c r="G16" s="8">
         <v>0</v>
       </c>
       <c r="H16" s="8">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="I16" s="8">
-        <v>20.55</v>
+        <v>21.19</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -984,28 +984,28 @@
         <v>23</v>
       </c>
       <c r="B17" s="8">
-        <v>11.12</v>
+        <v>11.04</v>
       </c>
       <c r="C17" s="8">
-        <v>8.11</v>
+        <v>8.15</v>
       </c>
       <c r="D17" s="8">
-        <v>18.77</v>
+        <v>18.809999999999999</v>
       </c>
       <c r="E17" s="8">
-        <v>41.48</v>
+        <v>41.28</v>
       </c>
       <c r="F17" s="8">
-        <v>-18.3</v>
+        <v>-18.64</v>
       </c>
       <c r="G17" s="8">
         <v>0</v>
       </c>
       <c r="H17" s="8">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="I17" s="8">
-        <v>23</v>
+        <v>24.36</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1013,28 +1013,28 @@
         <v>24</v>
       </c>
       <c r="B18" s="8">
-        <v>10</v>
+        <v>9.99</v>
       </c>
       <c r="C18" s="8">
-        <v>9.09</v>
+        <v>9.1199999999999992</v>
       </c>
       <c r="D18" s="8">
-        <v>18.899999999999999</v>
+        <v>18.89</v>
       </c>
       <c r="E18" s="8">
         <v>39.1</v>
       </c>
       <c r="F18" s="8">
-        <v>-18.79</v>
+        <v>-18.760000000000002</v>
       </c>
       <c r="G18" s="8">
         <v>0</v>
       </c>
       <c r="H18" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="I18" s="8">
-        <v>31.99</v>
+        <v>33.479999999999997</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1042,19 +1042,19 @@
         <v>25</v>
       </c>
       <c r="B19" s="10">
-        <v>10.17</v>
+        <v>10.24</v>
       </c>
       <c r="C19" s="10">
-        <v>6.88</v>
+        <v>6.81</v>
       </c>
       <c r="D19" s="10">
-        <v>20.95</v>
+        <v>20.96</v>
       </c>
       <c r="E19" s="10">
-        <v>37.4</v>
+        <v>37.520000000000003</v>
       </c>
       <c r="F19" s="10">
-        <v>-23.36</v>
+        <v>-23.29</v>
       </c>
       <c r="G19" s="10">
         <v>0</v>
@@ -1063,7 +1063,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="10">
-        <v>41.51</v>
+        <v>41.66</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1071,19 +1071,19 @@
         <v>26</v>
       </c>
       <c r="B20" s="10">
-        <v>9.76</v>
+        <v>9.98</v>
       </c>
       <c r="C20" s="10">
-        <v>6.53</v>
+        <v>6.8</v>
       </c>
       <c r="D20" s="10">
-        <v>20.71</v>
+        <v>21.23</v>
       </c>
       <c r="E20" s="10">
-        <v>35.81</v>
+        <v>36.729999999999997</v>
       </c>
       <c r="F20" s="10">
-        <v>-23.27</v>
+        <v>-23.89</v>
       </c>
       <c r="G20" s="10">
         <v>0</v>
@@ -1092,7 +1092,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="10">
-        <v>53.23</v>
+        <v>49.76</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1106,13 +1106,13 @@
         <v>7.99</v>
       </c>
       <c r="D21" s="10">
-        <v>22.49</v>
+        <v>22.51</v>
       </c>
       <c r="E21" s="10">
-        <v>30.54</v>
+        <v>30.51</v>
       </c>
       <c r="F21" s="10">
-        <v>-33.51</v>
+        <v>-33.39</v>
       </c>
       <c r="G21" s="10">
         <v>0</v>
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="10">
-        <v>79.739999999999995</v>
+        <v>80.86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>